<commit_message>
Update Matriz de Responsabilidades.xlsx
Cambio de formato (word a excel)
</commit_message>
<xml_diff>
--- a/ADMINISTRACIÓN DE PROYECTOS/Planeación del proyecto/Anexos/Matriz de Responsabilidades.xlsx
+++ b/ADMINISTRACIÓN DE PROYECTOS/Planeación del proyecto/Anexos/Matriz de Responsabilidades.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\girl_\Documents\DistribuidoraMueblesMaravatio\ADMINISTRACIÓN DE PROYECTOS\Planeación del proyecto\Anexos\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="135" windowWidth="18915" windowHeight="9210" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18705" windowHeight="7395"/>
   </bookViews>
   <sheets>
     <sheet name="Plantilla Matriz Responsabilida" sheetId="1" r:id="rId1"/>
@@ -15,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="75">
   <si>
     <t>EDT</t>
   </si>
@@ -51,12 +56,6 @@
   </si>
   <si>
     <t>Auditorias Internas y Externas Completadas</t>
-  </si>
-  <si>
-    <t>Nombre de proyecto</t>
-  </si>
-  <si>
-    <t>Código identificador del proyecto</t>
   </si>
   <si>
     <t>C = Consultado</t>
@@ -120,15 +119,6 @@
     </r>
   </si>
   <si>
-    <t>Gerente del proyecto</t>
-  </si>
-  <si>
-    <t>Miembro del equipo</t>
-  </si>
-  <si>
-    <t>Interesado  (Stakeholder)</t>
-  </si>
-  <si>
     <t>R = Responsable de la ejecución</t>
   </si>
   <si>
@@ -213,6 +203,93 @@
   </si>
   <si>
     <t>Apoyo Educativo</t>
+  </si>
+  <si>
+    <t>Distribuidora de Muebles Maravatío</t>
+  </si>
+  <si>
+    <t>01_DMM</t>
+  </si>
+  <si>
+    <t>Interesados</t>
+  </si>
+  <si>
+    <t>JTALE (Administradora de Proyecto &amp; Analista)</t>
+  </si>
+  <si>
+    <t>TTP  (Diseñadora)</t>
+  </si>
+  <si>
+    <t>JLA (Programador)</t>
+  </si>
+  <si>
+    <t>SDJM(Tester)</t>
+  </si>
+  <si>
+    <t>DEFINICIÓN DE REQUERIMIENTOS</t>
+  </si>
+  <si>
+    <t>1.1.1</t>
+  </si>
+  <si>
+    <t>Análisis del problema</t>
+  </si>
+  <si>
+    <t>1.1.2</t>
+  </si>
+  <si>
+    <t>Recopilar información</t>
+  </si>
+  <si>
+    <t>1.1.3</t>
+  </si>
+  <si>
+    <t>Identificación de requerimientos</t>
+  </si>
+  <si>
+    <t>1.1.4</t>
+  </si>
+  <si>
+    <t>1.1.5</t>
+  </si>
+  <si>
+    <t>Análisis de los requerimientos</t>
+  </si>
+  <si>
+    <t>1.1.6</t>
+  </si>
+  <si>
+    <t>Representación de los requerimiento</t>
+  </si>
+  <si>
+    <t>1.1.7</t>
+  </si>
+  <si>
+    <t>Comunicación de los requerimientos</t>
+  </si>
+  <si>
+    <t>1.1.8</t>
+  </si>
+  <si>
+    <t>Validación de requerimientos</t>
+  </si>
+  <si>
+    <t>1.1.9</t>
+  </si>
+  <si>
+    <t>Generación del SRS</t>
+  </si>
+  <si>
+    <t>1.1.10</t>
+  </si>
+  <si>
+    <t>Firma del SRS</t>
+  </si>
+  <si>
+    <t>DISEÑO FUNCIONAL</t>
+  </si>
+  <si>
+    <t>q.</t>
   </si>
 </sst>
 </file>
@@ -285,7 +362,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -316,8 +393,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.39994506668294322"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="20">
+  <borders count="22">
     <border>
       <left/>
       <right/>
@@ -552,11 +635,37 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -697,10 +806,6 @@
       <alignment vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -718,6 +823,42 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="9" fontId="6" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -734,6 +875,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -742,20 +886,20 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>695326</xdr:colOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>47624</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>52298</xdr:rowOff>
+      <xdr:rowOff>38099</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>790576</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>135972</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 1" descr="C:\Users\francysr\Desktop\logo_PM4R Cloud.png"/>
+        <xdr:cNvPr id="4" name="Picture 1"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -768,15 +912,14 @@
             </a:ext>
           </a:extLst>
         </a:blip>
-        <a:srcRect/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="1676401" y="52298"/>
-          <a:ext cx="1181100" cy="464674"/>
+          <a:off x="47624" y="38099"/>
+          <a:ext cx="1047751" cy="981076"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -901,7 +1044,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -936,7 +1079,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1145,30 +1288,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K32"/>
+  <dimension ref="A1:I32"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" style="1"/>
+    <col min="1" max="1" width="11.42578125" style="1" customWidth="1"/>
     <col min="2" max="2" width="3.28515625" customWidth="1"/>
     <col min="3" max="3" width="16.28515625" customWidth="1"/>
-    <col min="4" max="4" width="32.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="47.42578125" customWidth="1"/>
     <col min="5" max="5" width="16.28515625" customWidth="1"/>
-    <col min="6" max="6" width="13.28515625" customWidth="1"/>
-    <col min="7" max="8" width="13.28515625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="14.28515625" customWidth="1"/>
-    <col min="10" max="10" width="14.85546875" customWidth="1"/>
-    <col min="11" max="11" width="3.28515625" customWidth="1"/>
+    <col min="6" max="6" width="15.42578125" customWidth="1"/>
+    <col min="7" max="7" width="14.7109375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="14.140625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="3.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:11" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="2:11" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="2:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:9" s="1" customFormat="1" ht="80.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:9" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="2:9" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="2:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B4" s="2"/>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
@@ -1176,25 +1318,21 @@
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-      <c r="K4" s="4"/>
-    </row>
-    <row r="5" spans="2:11" ht="21" x14ac:dyDescent="0.35">
+      <c r="I4" s="4"/>
+    </row>
+    <row r="5" spans="2:9" ht="21" x14ac:dyDescent="0.35">
       <c r="B5" s="5"/>
-      <c r="C5" s="48" t="s">
+      <c r="C5" s="47" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="48"/>
-      <c r="E5" s="48"/>
-      <c r="F5" s="48"/>
-      <c r="G5" s="48"/>
-      <c r="H5" s="48"/>
-      <c r="I5" s="48"/>
-      <c r="J5" s="48"/>
-      <c r="K5" s="6"/>
-    </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="D5" s="47"/>
+      <c r="E5" s="47"/>
+      <c r="F5" s="47"/>
+      <c r="G5" s="47"/>
+      <c r="H5" s="47"/>
+      <c r="I5" s="6"/>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B6" s="5"/>
       <c r="C6" s="7"/>
       <c r="D6" s="7"/>
@@ -1202,43 +1340,37 @@
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
       <c r="H6" s="7"/>
-      <c r="I6" s="7"/>
-      <c r="J6" s="7"/>
-      <c r="K6" s="6"/>
-    </row>
-    <row r="7" spans="2:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I6" s="6"/>
+    </row>
+    <row r="7" spans="2:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B7" s="5"/>
       <c r="C7" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="50" t="s">
-        <v>12</v>
-      </c>
-      <c r="E7" s="51"/>
-      <c r="F7" s="51"/>
-      <c r="G7" s="51"/>
-      <c r="H7" s="51"/>
-      <c r="I7" s="51"/>
-      <c r="J7" s="52"/>
-      <c r="K7" s="6"/>
-    </row>
-    <row r="8" spans="2:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D7" s="49" t="s">
+        <v>46</v>
+      </c>
+      <c r="E7" s="50"/>
+      <c r="F7" s="50"/>
+      <c r="G7" s="50"/>
+      <c r="H7" s="50"/>
+      <c r="I7" s="6"/>
+    </row>
+    <row r="8" spans="2:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B8" s="5"/>
       <c r="C8" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="50" t="s">
-        <v>13</v>
-      </c>
-      <c r="E8" s="51"/>
-      <c r="F8" s="51"/>
-      <c r="G8" s="51"/>
-      <c r="H8" s="51"/>
-      <c r="I8" s="51"/>
-      <c r="J8" s="52"/>
-      <c r="K8" s="6"/>
-    </row>
-    <row r="9" spans="2:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D8" s="49" t="s">
+        <v>47</v>
+      </c>
+      <c r="E8" s="50"/>
+      <c r="F8" s="50"/>
+      <c r="G8" s="50"/>
+      <c r="H8" s="50"/>
+      <c r="I8" s="6"/>
+    </row>
+    <row r="9" spans="2:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B9" s="5"/>
       <c r="C9" s="7"/>
       <c r="D9" s="7"/>
@@ -1246,53 +1378,43 @@
       <c r="F9" s="7"/>
       <c r="G9" s="7"/>
       <c r="H9" s="7"/>
-      <c r="I9" s="7"/>
-      <c r="J9" s="7"/>
-      <c r="K9" s="6"/>
-    </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="I9" s="6"/>
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B10" s="5"/>
-      <c r="C10" s="49" t="s">
+      <c r="C10" s="52" t="s">
         <v>0</v>
       </c>
-      <c r="D10" s="49" t="s">
-        <v>23</v>
-      </c>
-      <c r="E10" s="47" t="s">
-        <v>25</v>
-      </c>
-      <c r="F10" s="47"/>
-      <c r="G10" s="47"/>
-      <c r="H10" s="47"/>
-      <c r="I10" s="47"/>
-      <c r="J10" s="47"/>
-      <c r="K10" s="6"/>
-    </row>
-    <row r="11" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="D10" s="52" t="s">
+        <v>21</v>
+      </c>
+      <c r="E10" s="54" t="s">
+        <v>48</v>
+      </c>
+      <c r="F10" s="55"/>
+      <c r="G10" s="55"/>
+      <c r="H10" s="55"/>
+      <c r="I10" s="6"/>
+    </row>
+    <row r="11" spans="2:9" ht="60" x14ac:dyDescent="0.25">
       <c r="B11" s="5"/>
-      <c r="C11" s="49"/>
-      <c r="D11" s="49"/>
+      <c r="C11" s="53"/>
+      <c r="D11" s="53"/>
       <c r="E11" s="16" t="s">
-        <v>26</v>
+        <v>49</v>
       </c>
       <c r="F11" s="16" t="s">
-        <v>27</v>
+        <v>50</v>
       </c>
       <c r="G11" s="16" t="s">
-        <v>27</v>
+        <v>51</v>
       </c>
       <c r="H11" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="I11" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="J11" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="K11" s="6"/>
-    </row>
-    <row r="12" spans="2:11" s="1" customFormat="1" ht="6.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+      <c r="I11" s="6"/>
+    </row>
+    <row r="12" spans="2:9" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="5"/>
       <c r="C12" s="21"/>
       <c r="D12" s="21"/>
@@ -1300,195 +1422,209 @@
       <c r="F12" s="22"/>
       <c r="G12" s="22"/>
       <c r="H12" s="22"/>
-      <c r="I12" s="22"/>
-      <c r="J12" s="22"/>
-      <c r="K12" s="6"/>
-    </row>
-    <row r="13" spans="2:11" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="I12" s="6"/>
+    </row>
+    <row r="13" spans="2:9" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B13" s="5"/>
       <c r="C13" s="41" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D13" s="42" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E13" s="43" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="F13" s="44" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="G13" s="45" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="H13" s="45" t="s">
-        <v>30</v>
-      </c>
-      <c r="I13" s="46" t="s">
-        <v>30</v>
-      </c>
-      <c r="J13" s="46" t="s">
-        <v>30</v>
-      </c>
-      <c r="K13" s="6"/>
-    </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+      <c r="I13" s="6"/>
+    </row>
+    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B14" s="5"/>
-      <c r="C14" s="36"/>
-      <c r="D14" s="40"/>
+      <c r="C14" s="36">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D14" s="40" t="s">
+        <v>53</v>
+      </c>
       <c r="E14" s="38"/>
       <c r="F14" s="37"/>
       <c r="G14" s="39"/>
       <c r="H14" s="39"/>
-      <c r="I14" s="39"/>
-      <c r="J14" s="36"/>
-      <c r="K14" s="6"/>
-    </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="I14" s="6"/>
+    </row>
+    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B15" s="5"/>
-      <c r="C15" s="41"/>
-      <c r="D15" s="42"/>
+      <c r="C15" s="41" t="s">
+        <v>54</v>
+      </c>
+      <c r="D15" s="42" t="s">
+        <v>55</v>
+      </c>
       <c r="E15" s="43"/>
       <c r="F15" s="44"/>
       <c r="G15" s="45"/>
       <c r="H15" s="45"/>
-      <c r="I15" s="46"/>
-      <c r="J15" s="46"/>
-      <c r="K15" s="6"/>
-    </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="I15" s="6"/>
+    </row>
+    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B16" s="5"/>
-      <c r="C16" s="36"/>
-      <c r="D16" s="40"/>
+      <c r="C16" s="36" t="s">
+        <v>56</v>
+      </c>
+      <c r="D16" s="40" t="s">
+        <v>57</v>
+      </c>
       <c r="E16" s="38"/>
       <c r="F16" s="37"/>
       <c r="G16" s="39"/>
       <c r="H16" s="39"/>
-      <c r="I16" s="39"/>
-      <c r="J16" s="36"/>
-      <c r="K16" s="6"/>
-    </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="I16" s="6"/>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B17" s="5"/>
-      <c r="C17" s="41"/>
-      <c r="D17" s="42"/>
+      <c r="C17" s="41" t="s">
+        <v>58</v>
+      </c>
+      <c r="D17" s="42" t="s">
+        <v>59</v>
+      </c>
       <c r="E17" s="43"/>
       <c r="F17" s="44"/>
       <c r="G17" s="45"/>
       <c r="H17" s="45"/>
-      <c r="I17" s="46"/>
-      <c r="J17" s="46"/>
-      <c r="K17" s="6"/>
-    </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="I17" s="6"/>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B18" s="5"/>
-      <c r="C18" s="36"/>
-      <c r="D18" s="40"/>
+      <c r="C18" s="36" t="s">
+        <v>60</v>
+      </c>
+      <c r="D18" s="40" t="s">
+        <v>74</v>
+      </c>
       <c r="E18" s="38"/>
       <c r="F18" s="37"/>
       <c r="G18" s="39"/>
       <c r="H18" s="39"/>
-      <c r="I18" s="39"/>
-      <c r="J18" s="36"/>
-      <c r="K18" s="6"/>
-    </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="I18" s="6"/>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B19" s="5"/>
-      <c r="C19" s="41"/>
-      <c r="D19" s="42"/>
-      <c r="E19" s="43"/>
-      <c r="F19" s="44"/>
-      <c r="G19" s="45"/>
-      <c r="H19" s="45"/>
-      <c r="I19" s="46"/>
-      <c r="J19" s="46"/>
-      <c r="K19" s="6"/>
-    </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C19" s="36" t="s">
+        <v>61</v>
+      </c>
+      <c r="D19" s="40" t="s">
+        <v>62</v>
+      </c>
+      <c r="E19" s="38"/>
+      <c r="F19" s="37"/>
+      <c r="G19" s="39"/>
+      <c r="H19" s="39"/>
+      <c r="I19" s="6"/>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B20" s="5"/>
-      <c r="C20" s="36"/>
-      <c r="D20" s="40"/>
-      <c r="E20" s="38"/>
-      <c r="F20" s="37"/>
-      <c r="G20" s="39"/>
-      <c r="H20" s="39"/>
-      <c r="I20" s="39"/>
-      <c r="J20" s="36"/>
-      <c r="K20" s="6"/>
-    </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C20" s="41" t="s">
+        <v>63</v>
+      </c>
+      <c r="D20" s="42" t="s">
+        <v>64</v>
+      </c>
+      <c r="E20" s="43"/>
+      <c r="F20" s="44"/>
+      <c r="G20" s="45"/>
+      <c r="H20" s="45"/>
+      <c r="I20" s="6"/>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B21" s="5"/>
-      <c r="C21" s="41"/>
-      <c r="D21" s="42"/>
-      <c r="E21" s="43"/>
-      <c r="F21" s="44"/>
-      <c r="G21" s="45"/>
-      <c r="H21" s="45"/>
-      <c r="I21" s="46"/>
-      <c r="J21" s="46"/>
-      <c r="K21" s="6"/>
-    </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C21" s="36" t="s">
+        <v>65</v>
+      </c>
+      <c r="D21" s="40" t="s">
+        <v>66</v>
+      </c>
+      <c r="E21" s="38"/>
+      <c r="F21" s="37"/>
+      <c r="G21" s="39"/>
+      <c r="H21" s="39"/>
+      <c r="I21" s="6"/>
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B22" s="5"/>
-      <c r="C22" s="36"/>
-      <c r="D22" s="40"/>
-      <c r="E22" s="38"/>
-      <c r="F22" s="37"/>
-      <c r="G22" s="39"/>
-      <c r="H22" s="39"/>
-      <c r="I22" s="39"/>
-      <c r="J22" s="36"/>
-      <c r="K22" s="6"/>
-    </row>
-    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C22" s="41" t="s">
+        <v>67</v>
+      </c>
+      <c r="D22" s="42" t="s">
+        <v>68</v>
+      </c>
+      <c r="E22" s="43"/>
+      <c r="F22" s="44"/>
+      <c r="G22" s="45"/>
+      <c r="H22" s="45"/>
+      <c r="I22" s="6"/>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B23" s="5"/>
-      <c r="C23" s="41"/>
-      <c r="D23" s="42"/>
-      <c r="E23" s="43"/>
-      <c r="F23" s="44"/>
-      <c r="G23" s="45"/>
-      <c r="H23" s="45"/>
-      <c r="I23" s="46"/>
-      <c r="J23" s="46"/>
-      <c r="K23" s="6"/>
-    </row>
-    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C23" s="36" t="s">
+        <v>69</v>
+      </c>
+      <c r="D23" s="40" t="s">
+        <v>70</v>
+      </c>
+      <c r="E23" s="38"/>
+      <c r="F23" s="37"/>
+      <c r="G23" s="39"/>
+      <c r="H23" s="39"/>
+      <c r="I23" s="6"/>
+    </row>
+    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B24" s="5"/>
-      <c r="C24" s="36"/>
-      <c r="D24" s="40"/>
-      <c r="E24" s="38"/>
-      <c r="F24" s="37"/>
-      <c r="G24" s="39"/>
-      <c r="H24" s="39"/>
-      <c r="I24" s="39"/>
-      <c r="J24" s="36"/>
-      <c r="K24" s="6"/>
-    </row>
-    <row r="25" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C24" s="41" t="s">
+        <v>71</v>
+      </c>
+      <c r="D24" s="42" t="s">
+        <v>72</v>
+      </c>
+      <c r="E24" s="43"/>
+      <c r="F24" s="44"/>
+      <c r="G24" s="45"/>
+      <c r="H24" s="45"/>
+      <c r="I24" s="6"/>
+    </row>
+    <row r="25" spans="2:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B25" s="5"/>
-      <c r="C25" s="41"/>
-      <c r="D25" s="42"/>
-      <c r="E25" s="43"/>
-      <c r="F25" s="44"/>
-      <c r="G25" s="45"/>
-      <c r="H25" s="45"/>
-      <c r="I25" s="46"/>
-      <c r="J25" s="46"/>
-      <c r="K25" s="6"/>
-    </row>
-    <row r="26" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C25" s="56">
+        <v>1.2</v>
+      </c>
+      <c r="D25" s="57" t="s">
+        <v>73</v>
+      </c>
+      <c r="E25" s="58"/>
+      <c r="F25" s="59"/>
+      <c r="G25" s="60"/>
+      <c r="H25" s="60"/>
+      <c r="I25" s="6"/>
+    </row>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B26" s="5"/>
-      <c r="C26" s="36"/>
-      <c r="D26" s="40"/>
-      <c r="E26" s="38"/>
-      <c r="F26" s="37"/>
-      <c r="G26" s="39"/>
-      <c r="H26" s="39"/>
-      <c r="I26" s="39"/>
-      <c r="J26" s="36"/>
-      <c r="K26" s="6"/>
-    </row>
-    <row r="27" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C26" s="61"/>
+      <c r="D26" s="61"/>
+      <c r="E26" s="61"/>
+      <c r="F26" s="61"/>
+      <c r="G26" s="61"/>
+      <c r="H26" s="61"/>
+      <c r="I26" s="6"/>
+    </row>
+    <row r="27" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B27" s="8"/>
       <c r="C27" s="9"/>
       <c r="D27" s="9"/>
@@ -1496,48 +1632,65 @@
       <c r="F27" s="9"/>
       <c r="G27" s="9"/>
       <c r="H27" s="9"/>
-      <c r="I27" s="9"/>
-      <c r="J27" s="9"/>
-      <c r="K27" s="10"/>
-    </row>
-    <row r="28" spans="2:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="I27" s="10"/>
+    </row>
+    <row r="28" spans="2:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+    </row>
+    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B29" s="1"/>
       <c r="C29" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E29" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="30" spans="2:11" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F29" s="1"/>
+    </row>
+    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B30" s="1"/>
       <c r="C30" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E30" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="31" spans="2:11" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F30" s="1"/>
+    </row>
+    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B31" s="1"/>
       <c r="C31" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E31" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="32" spans="2:11" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F31" s="1"/>
+    </row>
+    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B32" s="1"/>
       <c r="C32" s="1" t="s">
-        <v>15</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+      <c r="F32" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="E10:J10"/>
-    <mergeCell ref="C5:J5"/>
+    <mergeCell ref="E10:H10"/>
+    <mergeCell ref="C5:H5"/>
     <mergeCell ref="D10:D11"/>
     <mergeCell ref="C10:C11"/>
-    <mergeCell ref="D7:J7"/>
-    <mergeCell ref="D8:J8"/>
+    <mergeCell ref="D7:H7"/>
+    <mergeCell ref="D8:H8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="82" orientation="portrait" r:id="rId1"/>
@@ -1549,8 +1702,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:N41"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9:M9"/>
+    <sheetView showGridLines="0" topLeftCell="C7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1586,18 +1739,18 @@
     </row>
     <row r="6" spans="3:14" ht="21" x14ac:dyDescent="0.35">
       <c r="C6" s="5"/>
-      <c r="D6" s="48" t="s">
+      <c r="D6" s="47" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="48"/>
-      <c r="F6" s="48"/>
-      <c r="G6" s="48"/>
-      <c r="H6" s="48"/>
-      <c r="I6" s="48"/>
-      <c r="J6" s="48"/>
-      <c r="K6" s="48"/>
-      <c r="L6" s="48"/>
-      <c r="M6" s="48"/>
+      <c r="E6" s="47"/>
+      <c r="F6" s="47"/>
+      <c r="G6" s="47"/>
+      <c r="H6" s="47"/>
+      <c r="I6" s="47"/>
+      <c r="J6" s="47"/>
+      <c r="K6" s="47"/>
+      <c r="L6" s="47"/>
+      <c r="M6" s="47"/>
       <c r="N6" s="6"/>
     </row>
     <row r="7" spans="3:14" x14ac:dyDescent="0.25">
@@ -1619,17 +1772,17 @@
       <c r="D8" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="E8" s="50" t="s">
-        <v>50</v>
-      </c>
-      <c r="F8" s="51"/>
-      <c r="G8" s="51"/>
-      <c r="H8" s="51"/>
-      <c r="I8" s="51"/>
-      <c r="J8" s="51"/>
-      <c r="K8" s="51"/>
-      <c r="L8" s="51"/>
-      <c r="M8" s="52"/>
+      <c r="E8" s="49" t="s">
+        <v>45</v>
+      </c>
+      <c r="F8" s="50"/>
+      <c r="G8" s="50"/>
+      <c r="H8" s="50"/>
+      <c r="I8" s="50"/>
+      <c r="J8" s="50"/>
+      <c r="K8" s="50"/>
+      <c r="L8" s="50"/>
+      <c r="M8" s="51"/>
       <c r="N8" s="6"/>
     </row>
     <row r="9" spans="3:14" x14ac:dyDescent="0.25">
@@ -1637,17 +1790,17 @@
       <c r="D9" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="E9" s="50" t="s">
-        <v>49</v>
-      </c>
-      <c r="F9" s="51"/>
-      <c r="G9" s="51"/>
-      <c r="H9" s="51"/>
-      <c r="I9" s="51"/>
-      <c r="J9" s="51"/>
-      <c r="K9" s="51"/>
-      <c r="L9" s="51"/>
-      <c r="M9" s="52"/>
+      <c r="E9" s="49" t="s">
+        <v>44</v>
+      </c>
+      <c r="F9" s="50"/>
+      <c r="G9" s="50"/>
+      <c r="H9" s="50"/>
+      <c r="I9" s="50"/>
+      <c r="J9" s="50"/>
+      <c r="K9" s="50"/>
+      <c r="L9" s="50"/>
+      <c r="M9" s="51"/>
       <c r="N9" s="6"/>
     </row>
     <row r="10" spans="3:14" x14ac:dyDescent="0.25">
@@ -1666,55 +1819,55 @@
     </row>
     <row r="11" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C11" s="5"/>
-      <c r="D11" s="49" t="s">
+      <c r="D11" s="48" t="s">
         <v>0</v>
       </c>
-      <c r="E11" s="49" t="s">
+      <c r="E11" s="48" t="s">
+        <v>21</v>
+      </c>
+      <c r="F11" s="46" t="s">
         <v>23</v>
       </c>
-      <c r="F11" s="47" t="s">
-        <v>25</v>
-      </c>
-      <c r="G11" s="47"/>
-      <c r="H11" s="47"/>
-      <c r="I11" s="47"/>
-      <c r="J11" s="47"/>
-      <c r="K11" s="47"/>
-      <c r="L11" s="47"/>
-      <c r="M11" s="47"/>
+      <c r="G11" s="46"/>
+      <c r="H11" s="46"/>
+      <c r="I11" s="46"/>
+      <c r="J11" s="46"/>
+      <c r="K11" s="46"/>
+      <c r="L11" s="46"/>
+      <c r="M11" s="46"/>
       <c r="N11" s="6"/>
     </row>
     <row r="12" spans="3:14" ht="45" x14ac:dyDescent="0.25">
       <c r="C12" s="5"/>
-      <c r="D12" s="49"/>
-      <c r="E12" s="49"/>
+      <c r="D12" s="48"/>
+      <c r="E12" s="48"/>
       <c r="F12" s="16" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="G12" s="16" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="H12" s="16" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="I12" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="J12" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="J12" s="16" t="s">
-        <v>40</v>
-      </c>
       <c r="K12" s="16" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="L12" s="16" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="M12" s="16" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="N12" s="6"/>
     </row>
-    <row r="13" spans="3:14" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="3:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C13" s="5"/>
       <c r="D13" s="21"/>
       <c r="E13" s="21"/>
@@ -1734,7 +1887,7 @@
         <v>1</v>
       </c>
       <c r="E14" s="26" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="F14" s="27"/>
       <c r="G14" s="28"/>
@@ -1780,7 +1933,7 @@
         <v>2</v>
       </c>
       <c r="E16" s="32" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="F16" s="33"/>
       <c r="G16" s="34"/>
@@ -1798,7 +1951,7 @@
         <v>2.1</v>
       </c>
       <c r="E17" s="40" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="F17" s="38" t="s">
         <v>2</v>
@@ -1807,7 +1960,7 @@
       <c r="H17" s="39"/>
       <c r="I17" s="39"/>
       <c r="J17" s="39" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="K17" s="36"/>
       <c r="L17" s="37" t="s">
@@ -1822,7 +1975,7 @@
         <v>3</v>
       </c>
       <c r="E18" s="18" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="F18" s="24"/>
       <c r="G18" s="19"/>
@@ -1869,7 +2022,7 @@
         <v>10</v>
       </c>
       <c r="F20" s="38" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="G20" s="37" t="s">
         <v>1</v>
@@ -1892,7 +2045,7 @@
         <v>4</v>
       </c>
       <c r="E21" s="18" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="F21" s="24"/>
       <c r="G21" s="19"/>
@@ -1930,16 +2083,26 @@
     </row>
     <row r="23" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C23" s="8"/>
-      <c r="D23" s="9"/>
-      <c r="E23" s="9"/>
-      <c r="F23" s="9"/>
-      <c r="G23" s="9"/>
-      <c r="H23" s="9"/>
-      <c r="I23" s="9"/>
-      <c r="J23" s="9"/>
-      <c r="K23" s="9"/>
-      <c r="L23" s="9"/>
-      <c r="M23" s="9"/>
+      <c r="D23" s="36">
+        <v>5.3</v>
+      </c>
+      <c r="E23" s="40" t="s">
+        <v>11</v>
+      </c>
+      <c r="F23" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="G23" s="37"/>
+      <c r="H23" s="39" t="s">
+        <v>1</v>
+      </c>
+      <c r="I23" s="39"/>
+      <c r="J23" s="39"/>
+      <c r="K23" s="36"/>
+      <c r="L23" s="37" t="s">
+        <v>2</v>
+      </c>
+      <c r="M23" s="38"/>
       <c r="N23" s="10"/>
     </row>
     <row r="24" spans="2:14" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -1976,34 +2139,34 @@
     <row r="27" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B27" s="7"/>
       <c r="D27" s="1" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
     </row>
     <row r="28" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B28" s="7"/>
       <c r="D28" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
     </row>
     <row r="29" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B29" s="7"/>
       <c r="D29" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
     </row>
     <row r="30" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B30" s="7"/>
       <c r="D30" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="31" spans="2:14" x14ac:dyDescent="0.25">
@@ -2015,7 +2178,7 @@
     <row r="33" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E33" s="11"/>
       <c r="F33" s="13" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G33" s="13"/>
       <c r="H33" s="13"/>
@@ -2023,28 +2186,28 @@
     <row r="34" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E34" s="12"/>
       <c r="F34" s="14" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="G34" s="14"/>
       <c r="H34" s="14"/>
     </row>
     <row r="35" spans="5:8" x14ac:dyDescent="0.25">
       <c r="F35" s="12" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G35" s="12"/>
       <c r="H35" s="12"/>
     </row>
     <row r="36" spans="5:8" x14ac:dyDescent="0.25">
       <c r="F36" s="12" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G36" s="12"/>
       <c r="H36" s="12"/>
     </row>
     <row r="37" spans="5:8" x14ac:dyDescent="0.25">
       <c r="F37" s="12" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="G37" s="12"/>
       <c r="H37" s="12"/>

</xml_diff>

<commit_message>
Revisión de ortografía y formato
</commit_message>
<xml_diff>
--- a/ADMINISTRACIÓN DE PROYECTOS/Planeación del proyecto/Anexos/Matriz de Responsabilidades.xlsx
+++ b/ADMINISTRACIÓN DE PROYECTOS/Planeación del proyecto/Anexos/Matriz de Responsabilidades.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="529" uniqueCount="178">
   <si>
     <t>EDT</t>
   </si>
@@ -104,13 +104,7 @@
     <t>Interesados</t>
   </si>
   <si>
-    <t>JTALE (Administradora de Proyecto &amp; Analista)</t>
-  </si>
-  <si>
     <t>TTP  (Diseñadora)</t>
-  </si>
-  <si>
-    <t>JLA (Programador)</t>
   </si>
   <si>
     <t>DEFINICIÓN DE REQUERIMIENTOS</t>
@@ -375,24 +369,6 @@
     <t>Representación de los requerimientos</t>
   </si>
   <si>
-    <t>A / I</t>
-  </si>
-  <si>
-    <t>R / C</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> R</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> C / I</t>
-  </si>
-  <si>
-    <t>SDJM(Asesor)</t>
-  </si>
-  <si>
-    <t>SDJM               (Tester)</t>
-  </si>
-  <si>
     <t>1.6.6</t>
   </si>
   <si>
@@ -571,6 +547,33 @@
   </si>
   <si>
     <t>1.5.4</t>
+  </si>
+  <si>
+    <t>JLA (Programador  &amp; Ingeniero de validación y verificación)</t>
+  </si>
+  <si>
+    <t>SDJM               (Tester &amp; Documentador)</t>
+  </si>
+  <si>
+    <t>JTALE (Administradora de Proyecto, Analista &amp; Aseguradora de Calidad)</t>
+  </si>
+  <si>
+    <t>JFD                 (Asesor)</t>
+  </si>
+  <si>
+    <t>A / C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A </t>
+  </si>
+  <si>
+    <t>R / C / I</t>
+  </si>
+  <si>
+    <t>1.4.13</t>
+  </si>
+  <si>
+    <t>1.4.14</t>
   </si>
 </sst>
 </file>
@@ -863,7 +866,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -1031,6 +1034,34 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="9" fontId="8" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="8" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="9" fontId="8" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="8" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1052,33 +1083,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="9" fontId="8" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="14" fontId="8" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="9" fontId="8" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="14" fontId="8" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1450,8 +1456,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B82" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="E60" sqref="E60"/>
+    <sheetView tabSelected="1" topLeftCell="A72" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="D92" sqref="D92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1483,15 +1489,15 @@
     </row>
     <row r="5" spans="2:10" ht="21" x14ac:dyDescent="0.35">
       <c r="B5" s="5"/>
-      <c r="C5" s="53" t="s">
+      <c r="C5" s="60" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="53"/>
-      <c r="E5" s="53"/>
-      <c r="F5" s="53"/>
-      <c r="G5" s="53"/>
-      <c r="H5" s="53"/>
-      <c r="I5" s="53"/>
+      <c r="D5" s="60"/>
+      <c r="E5" s="60"/>
+      <c r="F5" s="60"/>
+      <c r="G5" s="60"/>
+      <c r="H5" s="60"/>
+      <c r="I5" s="60"/>
       <c r="J5" s="6"/>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.25">
@@ -1510,14 +1516,14 @@
       <c r="C7" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="56" t="s">
+      <c r="D7" s="63" t="s">
         <v>18</v>
       </c>
-      <c r="E7" s="57"/>
-      <c r="F7" s="57"/>
-      <c r="G7" s="57"/>
-      <c r="H7" s="57"/>
-      <c r="I7" s="57"/>
+      <c r="E7" s="64"/>
+      <c r="F7" s="64"/>
+      <c r="G7" s="64"/>
+      <c r="H7" s="64"/>
+      <c r="I7" s="64"/>
       <c r="J7" s="6"/>
     </row>
     <row r="8" spans="2:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1525,14 +1531,14 @@
       <c r="C8" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="56" t="s">
+      <c r="D8" s="63" t="s">
         <v>19</v>
       </c>
-      <c r="E8" s="57"/>
-      <c r="F8" s="57"/>
-      <c r="G8" s="57"/>
-      <c r="H8" s="57"/>
-      <c r="I8" s="57"/>
+      <c r="E8" s="64"/>
+      <c r="F8" s="64"/>
+      <c r="G8" s="64"/>
+      <c r="H8" s="64"/>
+      <c r="I8" s="64"/>
       <c r="J8" s="6"/>
     </row>
     <row r="9" spans="2:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1548,39 +1554,39 @@
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B10" s="5"/>
-      <c r="C10" s="54" t="s">
+      <c r="C10" s="61" t="s">
         <v>0</v>
       </c>
-      <c r="D10" s="54" t="s">
+      <c r="D10" s="61" t="s">
         <v>12</v>
       </c>
-      <c r="E10" s="51" t="s">
+      <c r="E10" s="58" t="s">
         <v>20</v>
       </c>
-      <c r="F10" s="52"/>
-      <c r="G10" s="52"/>
-      <c r="H10" s="52"/>
-      <c r="I10" s="52"/>
+      <c r="F10" s="59"/>
+      <c r="G10" s="59"/>
+      <c r="H10" s="59"/>
+      <c r="I10" s="59"/>
       <c r="J10" s="6"/>
     </row>
-    <row r="11" spans="2:10" ht="60" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:10" ht="90" x14ac:dyDescent="0.25">
       <c r="B11" s="5"/>
-      <c r="C11" s="55"/>
-      <c r="D11" s="55"/>
+      <c r="C11" s="62"/>
+      <c r="D11" s="62"/>
       <c r="E11" s="12" t="s">
+        <v>171</v>
+      </c>
+      <c r="F11" s="65" t="s">
         <v>21</v>
       </c>
-      <c r="F11" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="G11" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="H11" s="12" t="s">
-        <v>116</v>
-      </c>
-      <c r="I11" s="12" t="s">
-        <v>115</v>
+      <c r="G11" s="65" t="s">
+        <v>169</v>
+      </c>
+      <c r="H11" s="65" t="s">
+        <v>170</v>
+      </c>
+      <c r="I11" s="65" t="s">
+        <v>172</v>
       </c>
       <c r="J11" s="6"/>
     </row>
@@ -1616,21 +1622,21 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="D14" s="26" t="s">
-        <v>24</v>
-      </c>
-      <c r="E14" s="58" t="s">
-        <v>108</v>
-      </c>
-      <c r="F14" s="59" t="s">
-        <v>109</v>
-      </c>
-      <c r="G14" s="60" t="s">
-        <v>109</v>
-      </c>
-      <c r="H14" s="60" t="s">
-        <v>109</v>
-      </c>
-      <c r="I14" s="60" t="s">
+        <v>22</v>
+      </c>
+      <c r="E14" s="51" t="s">
+        <v>106</v>
+      </c>
+      <c r="F14" s="52" t="s">
+        <v>107</v>
+      </c>
+      <c r="G14" s="53" t="s">
+        <v>107</v>
+      </c>
+      <c r="H14" s="53" t="s">
+        <v>107</v>
+      </c>
+      <c r="I14" s="53" t="s">
         <v>4</v>
       </c>
       <c r="J14" s="6"/>
@@ -1638,22 +1644,22 @@
     <row r="15" spans="2:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B15" s="5"/>
       <c r="C15" s="35" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D15" s="36" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="E15" s="37" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F15" s="38" t="s">
-        <v>109</v>
+        <v>4</v>
       </c>
       <c r="G15" s="39" t="s">
-        <v>109</v>
+        <v>4</v>
       </c>
       <c r="H15" s="39" t="s">
-        <v>109</v>
+        <v>4</v>
       </c>
       <c r="I15" s="39" t="s">
         <v>4</v>
@@ -1663,13 +1669,13 @@
     <row r="16" spans="2:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B16" s="5"/>
       <c r="C16" s="40" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D16" s="41" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="E16" s="42" t="s">
-        <v>1</v>
+        <v>107</v>
       </c>
       <c r="F16" s="43" t="s">
         <v>2</v>
@@ -1678,20 +1684,18 @@
         <v>4</v>
       </c>
       <c r="H16" s="44" t="s">
-        <v>4</v>
-      </c>
-      <c r="I16" s="44" t="s">
-        <v>4</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="I16" s="44"/>
       <c r="J16" s="6"/>
     </row>
     <row r="17" spans="2:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B17" s="5"/>
       <c r="C17" s="35" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D17" s="36" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="E17" s="37" t="s">
         <v>1</v>
@@ -1713,13 +1717,13 @@
     <row r="18" spans="2:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B18" s="5"/>
       <c r="C18" s="40" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D18" s="41" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="E18" s="42" t="s">
-        <v>1</v>
+        <v>107</v>
       </c>
       <c r="F18" s="43" t="s">
         <v>2</v>
@@ -1728,7 +1732,7 @@
         <v>4</v>
       </c>
       <c r="H18" s="44" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I18" s="44" t="s">
         <v>4</v>
@@ -1738,13 +1742,13 @@
     <row r="19" spans="2:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B19" s="5"/>
       <c r="C19" s="35" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D19" s="36" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="E19" s="37" t="s">
-        <v>108</v>
+        <v>2</v>
       </c>
       <c r="F19" s="38" t="s">
         <v>4</v>
@@ -1753,7 +1757,7 @@
         <v>4</v>
       </c>
       <c r="H19" s="39" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I19" s="39" t="s">
         <v>4</v>
@@ -1763,38 +1767,38 @@
     <row r="20" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B20" s="5"/>
       <c r="C20" s="40" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D20" s="32" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E20" s="33" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F20" s="31" t="s">
-        <v>4</v>
+        <v>107</v>
       </c>
       <c r="G20" s="34" t="s">
-        <v>3</v>
+        <v>107</v>
       </c>
       <c r="H20" s="34" t="s">
-        <v>4</v>
+        <v>107</v>
       </c>
       <c r="I20" s="34" t="s">
-        <v>109</v>
+        <v>4</v>
       </c>
       <c r="J20" s="6"/>
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B21" s="5"/>
       <c r="C21" s="35" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D21" s="36" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E21" s="45" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F21" s="35" t="s">
         <v>4</v>
@@ -1806,42 +1810,42 @@
         <v>4</v>
       </c>
       <c r="I21" s="46" t="s">
-        <v>109</v>
+        <v>4</v>
       </c>
       <c r="J21" s="6"/>
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B22" s="5"/>
       <c r="C22" s="40" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D22" s="32" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E22" s="33" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F22" s="31" t="s">
-        <v>109</v>
+        <v>4</v>
       </c>
       <c r="G22" s="34" t="s">
-        <v>109</v>
+        <v>4</v>
       </c>
       <c r="H22" s="34" t="s">
-        <v>109</v>
+        <v>4</v>
       </c>
       <c r="I22" s="34" t="s">
-        <v>109</v>
+        <v>4</v>
       </c>
       <c r="J22" s="6"/>
     </row>
     <row r="23" spans="2:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B23" s="5"/>
       <c r="C23" s="35" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D23" s="30" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="E23" s="22" t="s">
         <v>1</v>
@@ -1850,10 +1854,10 @@
         <v>2</v>
       </c>
       <c r="G23" s="24" t="s">
-        <v>3</v>
+        <v>107</v>
       </c>
       <c r="H23" s="24" t="s">
-        <v>3</v>
+        <v>107</v>
       </c>
       <c r="I23" s="24" t="s">
         <v>4</v>
@@ -1863,22 +1867,22 @@
     <row r="24" spans="2:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="5"/>
       <c r="C24" s="40" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D24" s="47" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E24" s="48" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F24" s="40" t="s">
-        <v>109</v>
+        <v>4</v>
       </c>
       <c r="G24" s="49" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="H24" s="49" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="I24" s="49" t="s">
         <v>4</v>
@@ -1888,22 +1892,22 @@
     <row r="25" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B25" s="5"/>
       <c r="C25" s="35" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="D25" s="36" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E25" s="45" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F25" s="35" t="s">
-        <v>4</v>
+        <v>107</v>
       </c>
       <c r="G25" s="46" t="s">
-        <v>4</v>
+        <v>107</v>
       </c>
       <c r="H25" s="46" t="s">
-        <v>4</v>
+        <v>107</v>
       </c>
       <c r="I25" s="46" t="s">
         <v>4</v>
@@ -1913,13 +1917,13 @@
     <row r="26" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B26" s="5"/>
       <c r="C26" s="40" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="D26" s="32" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="E26" s="33" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F26" s="31" t="s">
         <v>4</v>
@@ -1938,13 +1942,13 @@
     <row r="27" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B27" s="5"/>
       <c r="C27" s="35" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="D27" s="36" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E27" s="45" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F27" s="35" t="s">
         <v>4</v>
@@ -1963,19 +1967,19 @@
     <row r="28" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B28" s="5"/>
       <c r="C28" s="40" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="D28" s="32" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E28" s="33" t="s">
-        <v>108</v>
+        <v>1</v>
       </c>
       <c r="F28" s="31" t="s">
         <v>4</v>
       </c>
       <c r="G28" s="34" t="s">
-        <v>4</v>
+        <v>173</v>
       </c>
       <c r="H28" s="34" t="s">
         <v>4</v>
@@ -1988,22 +1992,22 @@
     <row r="29" spans="2:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B29" s="5"/>
       <c r="C29" s="35" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="D29" s="30" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="E29" s="22" t="s">
-        <v>1</v>
+        <v>107</v>
       </c>
       <c r="F29" s="23" t="s">
         <v>2</v>
       </c>
       <c r="G29" s="24" t="s">
-        <v>4</v>
+        <v>107</v>
       </c>
       <c r="H29" s="24" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I29" s="24" t="s">
         <v>4</v>
@@ -2013,13 +2017,13 @@
     <row r="30" spans="2:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B30" s="5"/>
       <c r="C30" s="40" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="D30" s="32" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="E30" s="33" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F30" s="31" t="s">
         <v>4</v>
@@ -2038,22 +2042,22 @@
     <row r="31" spans="2:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B31" s="5"/>
       <c r="C31" s="35" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="D31" s="30" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="E31" s="22" t="s">
-        <v>108</v>
+        <v>2</v>
       </c>
       <c r="F31" s="23" t="s">
-        <v>109</v>
+        <v>4</v>
       </c>
       <c r="G31" s="24" t="s">
-        <v>109</v>
+        <v>4</v>
       </c>
       <c r="H31" s="24" t="s">
-        <v>109</v>
+        <v>1</v>
       </c>
       <c r="I31" s="24" t="s">
         <v>4</v>
@@ -2063,22 +2067,22 @@
     <row r="32" spans="2:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B32" s="5"/>
       <c r="C32" s="40" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="D32" s="32" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="E32" s="33" t="s">
-        <v>108</v>
+        <v>4</v>
       </c>
       <c r="F32" s="31" t="s">
-        <v>109</v>
+        <v>2</v>
       </c>
       <c r="G32" s="34" t="s">
-        <v>109</v>
+        <v>4</v>
       </c>
       <c r="H32" s="34" t="s">
-        <v>109</v>
+        <v>1</v>
       </c>
       <c r="I32" s="34" t="s">
         <v>4</v>
@@ -2088,16 +2092,16 @@
     <row r="33" spans="2:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B33" s="5"/>
       <c r="C33" s="35" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="D33" s="30" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="E33" s="22" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F33" s="23" t="s">
-        <v>4</v>
+        <v>107</v>
       </c>
       <c r="G33" s="24" t="s">
         <v>4</v>
@@ -2113,22 +2117,22 @@
     <row r="34" spans="2:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B34" s="5"/>
       <c r="C34" s="40" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="D34" s="32" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="E34" s="33" t="s">
-        <v>108</v>
+        <v>2</v>
       </c>
       <c r="F34" s="31" t="s">
-        <v>109</v>
+        <v>4</v>
       </c>
       <c r="G34" s="34" t="s">
-        <v>109</v>
+        <v>4</v>
       </c>
       <c r="H34" s="34" t="s">
-        <v>109</v>
+        <v>1</v>
       </c>
       <c r="I34" s="34" t="s">
         <v>4</v>
@@ -2138,13 +2142,13 @@
     <row r="35" spans="2:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B35" s="5"/>
       <c r="C35" s="35" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="D35" s="30" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="E35" s="22" t="s">
-        <v>1</v>
+        <v>107</v>
       </c>
       <c r="F35" s="23" t="s">
         <v>2</v>
@@ -2153,7 +2157,7 @@
         <v>4</v>
       </c>
       <c r="H35" s="24" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I35" s="24" t="s">
         <v>4</v>
@@ -2163,22 +2167,22 @@
     <row r="36" spans="2:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B36" s="5"/>
       <c r="C36" s="40" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="D36" s="32" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="E36" s="33" t="s">
-        <v>1</v>
+        <v>107</v>
       </c>
       <c r="F36" s="31" t="s">
         <v>2</v>
       </c>
       <c r="G36" s="34" t="s">
-        <v>109</v>
+        <v>4</v>
       </c>
       <c r="H36" s="34" t="s">
-        <v>109</v>
+        <v>1</v>
       </c>
       <c r="I36" s="34" t="s">
         <v>4</v>
@@ -2188,13 +2192,13 @@
     <row r="37" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B37" s="5"/>
       <c r="C37" s="35" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="D37" s="36" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E37" s="45" t="s">
-        <v>108</v>
+        <v>2</v>
       </c>
       <c r="F37" s="35" t="s">
         <v>4</v>
@@ -2203,7 +2207,7 @@
         <v>4</v>
       </c>
       <c r="H37" s="46" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I37" s="46" t="s">
         <v>4</v>
@@ -2213,38 +2217,38 @@
     <row r="38" spans="2:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B38" s="5"/>
       <c r="C38" s="40" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="D38" s="32" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E38" s="33" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F38" s="31" t="s">
-        <v>109</v>
+        <v>4</v>
       </c>
       <c r="G38" s="34" t="s">
-        <v>109</v>
+        <v>4</v>
       </c>
       <c r="H38" s="34" t="s">
-        <v>109</v>
+        <v>4</v>
       </c>
       <c r="I38" s="34" t="s">
-        <v>4</v>
+        <v>107</v>
       </c>
       <c r="J38" s="6"/>
     </row>
     <row r="39" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B39" s="5"/>
       <c r="C39" s="35" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="D39" s="30" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="E39" s="22" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F39" s="23" t="s">
         <v>4</v>
@@ -2256,29 +2260,29 @@
         <v>4</v>
       </c>
       <c r="I39" s="24" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="J39" s="6"/>
     </row>
     <row r="40" spans="2:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B40" s="5"/>
       <c r="C40" s="40" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="D40" s="32" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="E40" s="33" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F40" s="31" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="G40" s="34" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="H40" s="34" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="I40" s="34" t="s">
         <v>4</v>
@@ -2291,7 +2295,7 @@
         <v>1.2</v>
       </c>
       <c r="D41" s="20" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E41" s="27"/>
       <c r="F41" s="28"/>
@@ -2303,19 +2307,19 @@
     <row r="42" spans="2:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B42" s="5"/>
       <c r="C42" s="23" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D42" s="30" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E42" s="22" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="F42" s="23" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G42" s="24" t="s">
-        <v>1</v>
+        <v>107</v>
       </c>
       <c r="H42" s="24" t="s">
         <v>4</v>
@@ -2328,19 +2332,19 @@
     <row r="43" spans="2:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B43" s="5"/>
       <c r="C43" s="31" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D43" s="32" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E43" s="33" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F43" s="31" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G43" s="34" t="s">
-        <v>3</v>
+        <v>107</v>
       </c>
       <c r="H43" s="34" t="s">
         <v>4</v>
@@ -2353,44 +2357,44 @@
     <row r="44" spans="2:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B44" s="5"/>
       <c r="C44" s="23" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D44" s="30" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E44" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="F44" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="F44" s="23" t="s">
-        <v>112</v>
-      </c>
       <c r="G44" s="24" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="H44" s="24" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="I44" s="24" t="s">
-        <v>109</v>
+        <v>4</v>
       </c>
       <c r="J44" s="6"/>
     </row>
     <row r="45" spans="2:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B45" s="5"/>
       <c r="C45" s="31" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D45" s="32" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E45" s="33" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="F45" s="31" t="s">
         <v>4</v>
       </c>
       <c r="G45" s="34" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H45" s="34" t="s">
         <v>4</v>
@@ -2403,19 +2407,19 @@
     <row r="46" spans="2:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B46" s="5"/>
       <c r="C46" s="23" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D46" s="30" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E46" s="22" t="s">
-        <v>111</v>
+        <v>1</v>
       </c>
       <c r="F46" s="23" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G46" s="24" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H46" s="24" t="s">
         <v>4</v>
@@ -2428,44 +2432,44 @@
     <row r="47" spans="2:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B47" s="5"/>
       <c r="C47" s="31" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D47" s="32" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E47" s="33" t="s">
-        <v>109</v>
+        <v>1</v>
       </c>
       <c r="F47" s="31" t="s">
-        <v>108</v>
+        <v>174</v>
       </c>
       <c r="G47" s="34" t="s">
-        <v>109</v>
+        <v>4</v>
       </c>
       <c r="H47" s="34" t="s">
-        <v>109</v>
+        <v>4</v>
       </c>
       <c r="I47" s="34" t="s">
-        <v>109</v>
+        <v>4</v>
       </c>
       <c r="J47" s="6"/>
     </row>
     <row r="48" spans="2:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B48" s="5"/>
       <c r="C48" s="23" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D48" s="30" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E48" s="22" t="s">
-        <v>108</v>
+        <v>1</v>
       </c>
       <c r="F48" s="23" t="s">
         <v>4</v>
       </c>
       <c r="G48" s="24" t="s">
-        <v>4</v>
+        <v>173</v>
       </c>
       <c r="H48" s="24" t="s">
         <v>4</v>
@@ -2481,7 +2485,7 @@
         <v>1.3</v>
       </c>
       <c r="D49" s="20" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E49" s="27"/>
       <c r="F49" s="28"/>
@@ -2493,22 +2497,22 @@
     <row r="50" spans="2:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B50" s="5"/>
       <c r="C50" s="23" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D50" s="30" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E50" s="22" t="s">
         <v>2</v>
       </c>
       <c r="F50" s="23" t="s">
-        <v>114</v>
+        <v>1</v>
       </c>
       <c r="G50" s="24" t="s">
-        <v>113</v>
+        <v>3</v>
       </c>
       <c r="H50" s="24" t="s">
-        <v>109</v>
+        <v>4</v>
       </c>
       <c r="I50" s="24" t="s">
         <v>4</v>
@@ -2518,22 +2522,22 @@
     <row r="51" spans="2:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B51" s="5"/>
       <c r="C51" s="31" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D51" s="32" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E51" s="33" t="s">
-        <v>108</v>
+        <v>2</v>
       </c>
       <c r="F51" s="31" t="s">
-        <v>109</v>
+        <v>1</v>
       </c>
       <c r="G51" s="34" t="s">
-        <v>109</v>
+        <v>3</v>
       </c>
       <c r="H51" s="34" t="s">
-        <v>109</v>
+        <v>4</v>
       </c>
       <c r="I51" s="34" t="s">
         <v>4</v>
@@ -2543,22 +2547,22 @@
     <row r="52" spans="2:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B52" s="5"/>
       <c r="C52" s="23" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D52" s="30" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="E52" s="22" t="s">
-        <v>108</v>
+        <v>2</v>
       </c>
       <c r="F52" s="23" t="s">
-        <v>109</v>
+        <v>1</v>
       </c>
       <c r="G52" s="24" t="s">
-        <v>109</v>
+        <v>3</v>
       </c>
       <c r="H52" s="24" t="s">
-        <v>109</v>
+        <v>4</v>
       </c>
       <c r="I52" s="24" t="s">
         <v>4</v>
@@ -2568,19 +2572,19 @@
     <row r="53" spans="2:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B53" s="5"/>
       <c r="C53" s="31" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D53" s="32" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="E53" s="33" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F53" s="31" t="s">
-        <v>4</v>
+        <v>107</v>
       </c>
       <c r="G53" s="34" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H53" s="34" t="s">
         <v>4</v>
@@ -2593,19 +2597,19 @@
     <row r="54" spans="2:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B54" s="5"/>
       <c r="C54" s="23" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D54" s="30" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E54" s="22" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F54" s="23" t="s">
-        <v>4</v>
+        <v>107</v>
       </c>
       <c r="G54" s="24" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H54" s="24" t="s">
         <v>4</v>
@@ -2618,19 +2622,19 @@
     <row r="55" spans="2:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B55" s="5"/>
       <c r="C55" s="31" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D55" s="32" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E55" s="33" t="s">
-        <v>1</v>
+        <v>107</v>
       </c>
       <c r="F55" s="31" t="s">
-        <v>2</v>
+        <v>106</v>
       </c>
       <c r="G55" s="34" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H55" s="34" t="s">
         <v>4</v>
@@ -2643,13 +2647,13 @@
     <row r="56" spans="2:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B56" s="5"/>
       <c r="C56" s="23" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D56" s="30" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E56" s="22" t="s">
-        <v>109</v>
+        <v>4</v>
       </c>
       <c r="F56" s="23" t="s">
         <v>1</v>
@@ -2658,7 +2662,7 @@
         <v>2</v>
       </c>
       <c r="H56" s="24" t="s">
-        <v>109</v>
+        <v>4</v>
       </c>
       <c r="I56" s="24" t="s">
         <v>4</v>
@@ -2668,22 +2672,22 @@
     <row r="57" spans="2:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B57" s="5"/>
       <c r="C57" s="31" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D57" s="32" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E57" s="33" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="F57" s="31" t="s">
-        <v>1</v>
+        <v>106</v>
       </c>
       <c r="G57" s="34" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H57" s="34" t="s">
-        <v>109</v>
+        <v>4</v>
       </c>
       <c r="I57" s="34" t="s">
         <v>4</v>
@@ -2693,22 +2697,22 @@
     <row r="58" spans="2:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B58" s="5"/>
       <c r="C58" s="23" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D58" s="30" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E58" s="22" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="F58" s="23" t="s">
-        <v>109</v>
+        <v>1</v>
       </c>
       <c r="G58" s="24" t="s">
-        <v>108</v>
+        <v>2</v>
       </c>
       <c r="H58" s="24" t="s">
-        <v>109</v>
+        <v>4</v>
       </c>
       <c r="I58" s="24" t="s">
         <v>4</v>
@@ -2718,22 +2722,22 @@
     <row r="59" spans="2:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B59" s="5"/>
       <c r="C59" s="31" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D59" s="32" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E59" s="33" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F59" s="31" t="s">
-        <v>4</v>
+        <v>107</v>
       </c>
       <c r="G59" s="34" t="s">
-        <v>4</v>
+        <v>107</v>
       </c>
       <c r="H59" s="34" t="s">
-        <v>4</v>
+        <v>107</v>
       </c>
       <c r="I59" s="34" t="s">
         <v>4</v>
@@ -2743,22 +2747,22 @@
     <row r="60" spans="2:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B60" s="5"/>
       <c r="C60" s="23" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
       <c r="D60" s="50" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E60" s="22" t="s">
+        <v>107</v>
+      </c>
+      <c r="F60" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="F60" s="23" t="s">
+      <c r="G60" s="24" t="s">
+        <v>107</v>
+      </c>
+      <c r="H60" s="24" t="s">
         <v>1</v>
-      </c>
-      <c r="G60" s="24" t="s">
-        <v>109</v>
-      </c>
-      <c r="H60" s="24" t="s">
-        <v>109</v>
       </c>
       <c r="I60" s="24" t="s">
         <v>4</v>
@@ -2768,13 +2772,13 @@
     <row r="61" spans="2:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B61" s="5"/>
       <c r="C61" s="31" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="D61" s="32" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E61" s="33" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F61" s="31" t="s">
         <v>4</v>
@@ -2786,7 +2790,7 @@
         <v>4</v>
       </c>
       <c r="I61" s="34" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="J61" s="6"/>
     </row>
@@ -2796,7 +2800,7 @@
         <v>1.4</v>
       </c>
       <c r="D62" s="20" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E62" s="27"/>
       <c r="F62" s="28"/>
@@ -2808,22 +2812,22 @@
     <row r="63" spans="2:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B63" s="5"/>
       <c r="C63" s="31" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D63" s="32" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E63" s="33" t="s">
-        <v>4</v>
+        <v>107</v>
       </c>
       <c r="F63" s="31" t="s">
         <v>4</v>
       </c>
       <c r="G63" s="34" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="H63" s="34" t="s">
-        <v>109</v>
+        <v>4</v>
       </c>
       <c r="I63" s="34" t="s">
         <v>4</v>
@@ -2833,16 +2837,16 @@
     <row r="64" spans="2:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B64" s="5"/>
       <c r="C64" s="23" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D64" s="30" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="E64" s="22" t="s">
-        <v>4</v>
+        <v>107</v>
       </c>
       <c r="F64" s="23" t="s">
-        <v>4</v>
+        <v>107</v>
       </c>
       <c r="G64" s="24" t="s">
         <v>1</v>
@@ -2858,16 +2862,16 @@
     <row r="65" spans="2:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B65" s="5"/>
       <c r="C65" s="31" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D65" s="32" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="E65" s="33" t="s">
-        <v>4</v>
+        <v>107</v>
       </c>
       <c r="F65" s="31" t="s">
-        <v>4</v>
+        <v>107</v>
       </c>
       <c r="G65" s="34" t="s">
         <v>1</v>
@@ -2883,16 +2887,16 @@
     <row r="66" spans="2:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B66" s="5"/>
       <c r="C66" s="23" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D66" s="30" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="E66" s="22" t="s">
-        <v>4</v>
+        <v>107</v>
       </c>
       <c r="F66" s="23" t="s">
-        <v>4</v>
+        <v>107</v>
       </c>
       <c r="G66" s="24" t="s">
         <v>1</v>
@@ -2908,16 +2912,16 @@
     <row r="67" spans="2:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B67" s="5"/>
       <c r="C67" s="31" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D67" s="32" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="E67" s="33" t="s">
-        <v>4</v>
+        <v>107</v>
       </c>
       <c r="F67" s="31" t="s">
-        <v>4</v>
+        <v>107</v>
       </c>
       <c r="G67" s="34" t="s">
         <v>1</v>
@@ -2933,16 +2937,16 @@
     <row r="68" spans="2:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B68" s="5"/>
       <c r="C68" s="23" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D68" s="30" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="E68" s="22" t="s">
-        <v>4</v>
+        <v>107</v>
       </c>
       <c r="F68" s="23" t="s">
-        <v>4</v>
+        <v>107</v>
       </c>
       <c r="G68" s="24" t="s">
         <v>1</v>
@@ -2958,16 +2962,16 @@
     <row r="69" spans="2:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B69" s="5"/>
       <c r="C69" s="31" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D69" s="32" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="E69" s="33" t="s">
-        <v>4</v>
+        <v>107</v>
       </c>
       <c r="F69" s="31" t="s">
-        <v>4</v>
+        <v>107</v>
       </c>
       <c r="G69" s="34" t="s">
         <v>1</v>
@@ -2983,22 +2987,22 @@
     <row r="70" spans="2:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B70" s="5"/>
       <c r="C70" s="23" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D70" s="30" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
       <c r="E70" s="22" t="s">
-        <v>4</v>
+        <v>107</v>
       </c>
       <c r="F70" s="23" t="s">
-        <v>4</v>
+        <v>107</v>
       </c>
       <c r="G70" s="24" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="H70" s="24" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="I70" s="24" t="s">
         <v>4</v>
@@ -3008,22 +3012,22 @@
     <row r="71" spans="2:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B71" s="5"/>
       <c r="C71" s="31" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D71" s="32" t="s">
-        <v>171</v>
+        <v>163</v>
       </c>
       <c r="E71" s="33" t="s">
-        <v>4</v>
+        <v>107</v>
       </c>
       <c r="F71" s="31" t="s">
-        <v>4</v>
+        <v>107</v>
       </c>
       <c r="G71" s="34" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="H71" s="34" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="I71" s="34" t="s">
         <v>4</v>
@@ -3033,22 +3037,22 @@
     <row r="72" spans="2:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B72" s="5"/>
       <c r="C72" s="23" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D72" s="30" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="E72" s="22" t="s">
-        <v>4</v>
+        <v>107</v>
       </c>
       <c r="F72" s="23" t="s">
-        <v>4</v>
+        <v>107</v>
       </c>
       <c r="G72" s="24" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="H72" s="24" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="I72" s="24" t="s">
         <v>4</v>
@@ -3058,22 +3062,22 @@
     <row r="73" spans="2:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B73" s="5"/>
       <c r="C73" s="31" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D73" s="32" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="E73" s="33" t="s">
-        <v>4</v>
+        <v>107</v>
       </c>
       <c r="F73" s="31" t="s">
-        <v>4</v>
+        <v>107</v>
       </c>
       <c r="G73" s="34" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="H73" s="34" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="I73" s="34" t="s">
         <v>4</v>
@@ -3082,21 +3086,23 @@
     </row>
     <row r="74" spans="2:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B74" s="5"/>
-      <c r="C74" s="23"/>
+      <c r="C74" s="23" t="s">
+        <v>91</v>
+      </c>
       <c r="D74" s="30" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
       <c r="E74" s="22" t="s">
-        <v>4</v>
+        <v>107</v>
       </c>
       <c r="F74" s="23" t="s">
-        <v>4</v>
+        <v>107</v>
       </c>
       <c r="G74" s="24" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="H74" s="24" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="I74" s="24" t="s">
         <v>4</v>
@@ -3105,21 +3111,23 @@
     </row>
     <row r="75" spans="2:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B75" s="5"/>
-      <c r="C75" s="31"/>
+      <c r="C75" s="31" t="s">
+        <v>176</v>
+      </c>
       <c r="D75" s="32" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
       <c r="E75" s="33" t="s">
-        <v>4</v>
+        <v>107</v>
       </c>
       <c r="F75" s="31" t="s">
-        <v>4</v>
+        <v>107</v>
       </c>
       <c r="G75" s="34" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="H75" s="34" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="I75" s="34" t="s">
         <v>4</v>
@@ -3129,25 +3137,25 @@
     <row r="76" spans="2:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B76" s="5"/>
       <c r="C76" s="23" t="s">
-        <v>93</v>
+        <v>177</v>
       </c>
       <c r="D76" s="30" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E76" s="22" t="s">
-        <v>2</v>
+        <v>106</v>
       </c>
       <c r="F76" s="23" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="G76" s="24" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="H76" s="24" t="s">
-        <v>1</v>
+        <v>107</v>
       </c>
       <c r="I76" s="24" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="J76" s="6"/>
     </row>
@@ -3157,7 +3165,7 @@
         <v>1.5</v>
       </c>
       <c r="D77" s="20" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E77" s="27"/>
       <c r="F77" s="28"/>
@@ -3169,24 +3177,24 @@
     <row r="78" spans="2:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B78" s="5"/>
       <c r="C78" s="31" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
       <c r="D78" s="32" t="s">
-        <v>133</v>
-      </c>
-      <c r="E78" s="62" t="s">
-        <v>108</v>
-      </c>
-      <c r="F78" s="63" t="s">
-        <v>4</v>
-      </c>
-      <c r="G78" s="64" t="s">
-        <v>4</v>
-      </c>
-      <c r="H78" s="64" t="s">
-        <v>4</v>
-      </c>
-      <c r="I78" s="64" t="s">
+        <v>125</v>
+      </c>
+      <c r="E78" s="55" t="s">
+        <v>107</v>
+      </c>
+      <c r="F78" s="56" t="s">
+        <v>107</v>
+      </c>
+      <c r="G78" s="57" t="s">
+        <v>107</v>
+      </c>
+      <c r="H78" s="57" t="s">
+        <v>106</v>
+      </c>
+      <c r="I78" s="57" t="s">
         <v>4</v>
       </c>
       <c r="J78" s="6"/>
@@ -3194,13 +3202,13 @@
     <row r="79" spans="2:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B79" s="5"/>
       <c r="C79" s="23" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="D79" s="30" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="E79" s="22" t="s">
-        <v>4</v>
+        <v>107</v>
       </c>
       <c r="F79" s="23" t="s">
         <v>4</v>
@@ -3209,7 +3217,7 @@
         <v>4</v>
       </c>
       <c r="H79" s="24" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="I79" s="24" t="s">
         <v>4</v>
@@ -3219,13 +3227,13 @@
     <row r="80" spans="2:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B80" s="5"/>
       <c r="C80" s="31" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
       <c r="D80" s="32" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E80" s="33" t="s">
-        <v>4</v>
+        <v>107</v>
       </c>
       <c r="F80" s="31" t="s">
         <v>4</v>
@@ -3234,7 +3242,7 @@
         <v>4</v>
       </c>
       <c r="H80" s="34" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="I80" s="34" t="s">
         <v>4</v>
@@ -3244,22 +3252,22 @@
     <row r="81" spans="2:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B81" s="5"/>
       <c r="C81" s="23" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="D81" s="30" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E81" s="22" t="s">
-        <v>4</v>
+        <v>173</v>
       </c>
       <c r="F81" s="23" t="s">
-        <v>4</v>
+        <v>107</v>
       </c>
       <c r="G81" s="24" t="s">
-        <v>4</v>
+        <v>107</v>
       </c>
       <c r="H81" s="24" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="I81" s="24" t="s">
         <v>4</v>
@@ -3272,7 +3280,7 @@
         <v>1.6</v>
       </c>
       <c r="D82" s="20" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E82" s="27"/>
       <c r="F82" s="28"/>
@@ -3284,24 +3292,24 @@
     <row r="83" spans="2:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B83" s="5"/>
       <c r="C83" s="31" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D83" s="32" t="s">
-        <v>121</v>
-      </c>
-      <c r="E83" s="62" t="s">
-        <v>108</v>
-      </c>
-      <c r="F83" s="63" t="s">
-        <v>4</v>
-      </c>
-      <c r="G83" s="64" t="s">
-        <v>4</v>
-      </c>
-      <c r="H83" s="64" t="s">
-        <v>4</v>
-      </c>
-      <c r="I83" s="64" t="s">
+        <v>113</v>
+      </c>
+      <c r="E83" s="55" t="s">
+        <v>2</v>
+      </c>
+      <c r="F83" s="56" t="s">
+        <v>4</v>
+      </c>
+      <c r="G83" s="57" t="s">
+        <v>4</v>
+      </c>
+      <c r="H83" s="57" t="s">
+        <v>1</v>
+      </c>
+      <c r="I83" s="57" t="s">
         <v>4</v>
       </c>
       <c r="J83" s="6"/>
@@ -3309,138 +3317,138 @@
     <row r="84" spans="2:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B84" s="5"/>
       <c r="C84" s="23" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D84" s="30" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E84" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="F84" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="F84" s="23" t="s">
-        <v>4</v>
-      </c>
       <c r="G84" s="24" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H84" s="24" t="s">
         <v>4</v>
       </c>
       <c r="I84" s="24" t="s">
-        <v>4</v>
+        <v>107</v>
       </c>
       <c r="J84" s="6"/>
     </row>
     <row r="85" spans="2:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B85" s="5"/>
       <c r="C85" s="31" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D85" s="32" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E85" s="33" t="s">
-        <v>109</v>
+        <v>1</v>
       </c>
       <c r="F85" s="31" t="s">
-        <v>109</v>
+        <v>4</v>
       </c>
       <c r="G85" s="34" t="s">
-        <v>109</v>
+        <v>4</v>
       </c>
       <c r="H85" s="34" t="s">
-        <v>108</v>
+        <v>2</v>
       </c>
       <c r="I85" s="34" t="s">
-        <v>1</v>
+        <v>107</v>
       </c>
       <c r="J85" s="6"/>
     </row>
     <row r="86" spans="2:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B86" s="5"/>
       <c r="C86" s="23" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D86" s="30" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E86" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="F86" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="G86" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="F86" s="23" t="s">
-        <v>109</v>
-      </c>
-      <c r="G86" s="24" t="s">
-        <v>1</v>
-      </c>
       <c r="H86" s="24" t="s">
-        <v>109</v>
+        <v>4</v>
       </c>
       <c r="I86" s="24" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="J86" s="6"/>
     </row>
     <row r="87" spans="2:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B87" s="5"/>
       <c r="C87" s="31" t="s">
-        <v>106</v>
-      </c>
-      <c r="D87" s="61" t="s">
-        <v>120</v>
+        <v>104</v>
+      </c>
+      <c r="D87" s="54" t="s">
+        <v>112</v>
       </c>
       <c r="E87" s="33" t="s">
+        <v>107</v>
+      </c>
+      <c r="F87" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="F87" s="31" t="s">
-        <v>109</v>
-      </c>
       <c r="G87" s="34" t="s">
+        <v>4</v>
+      </c>
+      <c r="H87" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="H87" s="34" t="s">
-        <v>109</v>
-      </c>
       <c r="I87" s="34" t="s">
-        <v>109</v>
+        <v>4</v>
       </c>
       <c r="J87" s="6"/>
     </row>
     <row r="88" spans="2:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B88" s="5"/>
       <c r="C88" s="23" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="D88" s="30" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E88" s="22" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F88" s="23" t="s">
-        <v>109</v>
+        <v>4</v>
       </c>
       <c r="G88" s="24" t="s">
-        <v>109</v>
+        <v>4</v>
       </c>
       <c r="H88" s="24" t="s">
-        <v>109</v>
+        <v>4</v>
       </c>
       <c r="I88" s="24" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="J88" s="6"/>
     </row>
     <row r="89" spans="2:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B89" s="5"/>
       <c r="C89" s="31" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="D89" s="32" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="E89" s="33" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F89" s="31" t="s">
         <v>4</v>
@@ -3452,32 +3460,32 @@
         <v>4</v>
       </c>
       <c r="I89" s="34" t="s">
-        <v>4</v>
+        <v>107</v>
       </c>
       <c r="J89" s="6"/>
     </row>
     <row r="90" spans="2:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B90" s="5"/>
       <c r="C90" s="23" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="D90" s="30" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="E90" s="22" t="s">
-        <v>108</v>
+        <v>2</v>
       </c>
       <c r="F90" s="23" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="G90" s="24" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="H90" s="24" t="s">
-        <v>109</v>
+        <v>175</v>
       </c>
       <c r="I90" s="24" t="s">
-        <v>109</v>
+        <v>4</v>
       </c>
       <c r="J90" s="6"/>
     </row>

</xml_diff>